<commit_message>
Global controls partially implemented.
</commit_message>
<xml_diff>
--- a/notebook/release_notes.xlsx
+++ b/notebook/release_notes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tpd0001/github/watch-wv/notebook/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28CBBCA2-8A8E-3E44-B5AB-C273A8C23758}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F024062A-5E33-A847-9772-7D5F501637BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="51740" yWindow="80" windowWidth="28040" windowHeight="17440" activeTab="1" xr2:uid="{4289006E-909A-254F-9CBF-40213D5D9E21}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" activeTab="1" xr2:uid="{4289006E-909A-254F-9CBF-40213D5D9E21}"/>
   </bookViews>
   <sheets>
     <sheet name="events" sheetId="2" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="37">
   <si>
     <t>DONE</t>
   </si>
@@ -143,6 +143,9 @@
   </si>
   <si>
     <t>Add tab for Ethical considerations of WW testing.</t>
+  </si>
+  <si>
+    <t>Deploy from github directly.</t>
   </si>
 </sst>
 </file>
@@ -625,10 +628,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B141715B-50BC-AB41-8F99-F7D389132E3C}">
-  <dimension ref="A1:F17"/>
+  <dimension ref="A1:F18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="21" x14ac:dyDescent="0.25"/>
@@ -818,6 +821,15 @@
       <c r="A15" s="5">
         <v>4</v>
       </c>
+      <c r="B15" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C15" s="3">
+        <v>44671</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>32</v>
+      </c>
       <c r="E15" s="2" t="s">
         <v>30</v>
       </c>
@@ -836,6 +848,14 @@
       </c>
       <c r="E17" s="2" t="s">
         <v>28</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="22" x14ac:dyDescent="0.25">
+      <c r="A18" s="5">
+        <v>9</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>36</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Data update 5/16 run.
</commit_message>
<xml_diff>
--- a/notebook/release_notes.xlsx
+++ b/notebook/release_notes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tpd0001/github/watch-wv/notebook/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F024062A-5E33-A847-9772-7D5F501637BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DAE77D10-27A8-AB49-85D8-7B45347D8061}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" activeTab="1" xr2:uid="{4289006E-909A-254F-9CBF-40213D5D9E21}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="42">
   <si>
     <t>DONE</t>
   </si>
@@ -55,9 +55,6 @@
     <t>Move date slider to overlay, remove from control panel.</t>
   </si>
   <si>
-    <t>Color map points by...?? Thinking about deviation from CI of past N samples. Daily? weekly? mean of past X?</t>
-  </si>
-  <si>
     <t>Status</t>
   </si>
   <si>
@@ -146,6 +143,24 @@
   </si>
   <si>
     <t>Deploy from github directly.</t>
+  </si>
+  <si>
+    <t>Color map points by alert status - combo of level and trend.</t>
+  </si>
+  <si>
+    <t>1.0.0</t>
+  </si>
+  <si>
+    <t>POSTPONED</t>
+  </si>
+  <si>
+    <t>WORKING</t>
+  </si>
+  <si>
+    <t>Tried numerous times but doesn't seem to work as advertised.</t>
+  </si>
+  <si>
+    <t>PENDING</t>
   </si>
 </sst>
 </file>
@@ -549,22 +564,22 @@
   <sheetData>
     <row r="1" spans="1:6" ht="22" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="E1" s="2" t="s">
-        <v>14</v>
-      </c>
       <c r="F1" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="44" x14ac:dyDescent="0.2">
@@ -572,16 +587,16 @@
         <v>44670</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C2" s="2">
         <v>0.9</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="66" x14ac:dyDescent="0.2">
@@ -589,19 +604,19 @@
         <v>44671</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C3" s="2">
         <v>0.9</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="22" x14ac:dyDescent="0.2">
@@ -609,16 +624,16 @@
         <v>44673</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C4" s="2">
         <v>1</v>
       </c>
       <c r="D4" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E4" s="2" t="s">
         <v>19</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>20</v>
       </c>
     </row>
   </sheetData>
@@ -631,13 +646,13 @@
   <dimension ref="A1:F18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="21" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10.83203125" style="5"/>
-    <col min="2" max="2" width="10.83203125" style="2"/>
+    <col min="2" max="2" width="22.83203125" style="2" customWidth="1"/>
     <col min="3" max="3" width="11.33203125" style="2" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11" style="2" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="62.33203125" style="2" customWidth="1"/>
@@ -647,22 +662,22 @@
   <sheetData>
     <row r="1" spans="1:6" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>12</v>
-      </c>
       <c r="E1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>9</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="22" x14ac:dyDescent="0.25">
@@ -676,7 +691,7 @@
         <v>44670</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>1</v>
@@ -693,7 +708,7 @@
         <v>44670</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E3" s="2" t="s">
         <v>3</v>
@@ -710,7 +725,7 @@
         <v>44670</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>4</v>
@@ -727,7 +742,7 @@
         <v>44670</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E5" s="2" t="s">
         <v>5</v>
@@ -737,8 +752,17 @@
       <c r="A6" s="5">
         <v>1</v>
       </c>
+      <c r="B6" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C6" s="3">
+        <v>44696</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>37</v>
+      </c>
       <c r="E6" s="2" t="s">
-        <v>6</v>
+        <v>36</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="22" x14ac:dyDescent="0.25">
@@ -746,7 +770,7 @@
         <v>1</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="22" x14ac:dyDescent="0.25">
@@ -754,18 +778,21 @@
         <v>2</v>
       </c>
       <c r="E8" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="F8" s="2" t="s">
         <v>22</v>
-      </c>
-      <c r="F8" s="2" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="44" x14ac:dyDescent="0.25">
       <c r="A9" s="5">
         <v>2</v>
       </c>
+      <c r="B9" s="2" t="s">
+        <v>38</v>
+      </c>
       <c r="E9" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="22" x14ac:dyDescent="0.25">
@@ -773,7 +800,7 @@
         <v>3</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="22" x14ac:dyDescent="0.25">
@@ -787,18 +814,21 @@
         <v>44670</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="22" x14ac:dyDescent="0.25">
       <c r="A12" s="5">
         <v>4</v>
       </c>
+      <c r="B12" s="2" t="s">
+        <v>39</v>
+      </c>
       <c r="E12" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="22" x14ac:dyDescent="0.25">
@@ -806,15 +836,21 @@
         <v>4</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" ht="22" x14ac:dyDescent="0.25">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="44" x14ac:dyDescent="0.25">
       <c r="A14" s="5">
         <v>4</v>
       </c>
+      <c r="B14" s="2" t="s">
+        <v>39</v>
+      </c>
       <c r="E14" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="22" x14ac:dyDescent="0.25">
@@ -828,16 +864,19 @@
         <v>44671</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="44" x14ac:dyDescent="0.25">
       <c r="A16" s="5">
         <v>5</v>
       </c>
+      <c r="B16" s="2" t="s">
+        <v>39</v>
+      </c>
       <c r="E16" s="2" t="s">
         <v>2</v>
       </c>
@@ -846,16 +885,28 @@
       <c r="A17" s="5">
         <v>7</v>
       </c>
+      <c r="B17" s="2" t="s">
+        <v>41</v>
+      </c>
       <c r="E17" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="22" x14ac:dyDescent="0.25">
       <c r="A18" s="5">
         <v>9</v>
       </c>
+      <c r="B18" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C18" s="3">
+        <v>44681</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>31</v>
+      </c>
       <c r="E18" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
New release notes addition.
</commit_message>
<xml_diff>
--- a/notebook/release_notes.xlsx
+++ b/notebook/release_notes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tpd0001/github/watch-wv/notebook/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17387282-16B2-4A44-9324-57709DA47B47}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F2691CB-C3F2-CF4B-89EC-B14740D2C2FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="23140" windowHeight="14180" activeTab="1" xr2:uid="{4289006E-909A-254F-9CBF-40213D5D9E21}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="57">
   <si>
     <t>DONE</t>
   </si>
@@ -205,6 +205,12 @@
   </si>
   <si>
     <t>master</t>
+  </si>
+  <si>
+    <t>Add capability for multiple pathogens.</t>
+  </si>
+  <si>
+    <t>multipath</t>
   </si>
 </sst>
 </file>
@@ -711,10 +717,10 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B141715B-50BC-AB41-8F99-F7D389132E3C}">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:G18"/>
+  <dimension ref="A1:G19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="21" x14ac:dyDescent="0.25"/>
@@ -828,9 +834,6 @@
       <c r="B7" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="C7" s="2" t="s">
-        <v>54</v>
-      </c>
       <c r="F7" s="2" t="s">
         <v>30</v>
       </c>
@@ -975,6 +978,20 @@
       </c>
       <c r="F18" s="2" t="s">
         <v>47</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="22" x14ac:dyDescent="0.25">
+      <c r="A19" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="F19" s="2" t="s">
+        <v>55</v>
       </c>
     </row>
   </sheetData>

</xml_diff>